<commit_message>
Changing plan and complete SRS
</commit_message>
<xml_diff>
--- a/Document/Planning.xlsx
+++ b/Document/Planning.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PythonProject\Senior Project\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD300A5B-70DD-441C-860E-2DE2826DBD09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F49FF0D-323C-4016-B7B8-21D65E10C37A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1164,22 +1164,19 @@
     <xf numFmtId="0" fontId="4" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="19" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="19" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="19" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1191,14 +1188,17 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="19" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="19" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="19" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1800,8 +1800,8 @@
   </sheetPr>
   <dimension ref="A1:BL42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A2" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A16" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1827,28 +1827,28 @@
       <c r="E1" s="20"/>
       <c r="F1" s="21"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="129" t="s">
+      <c r="I1" s="128" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="130"/>
-      <c r="K1" s="130"/>
-      <c r="L1" s="130"/>
-      <c r="M1" s="130"/>
-      <c r="N1" s="130"/>
-      <c r="O1" s="130"/>
+      <c r="J1" s="129"/>
+      <c r="K1" s="129"/>
+      <c r="L1" s="129"/>
+      <c r="M1" s="129"/>
+      <c r="N1" s="129"/>
+      <c r="O1" s="129"/>
       <c r="P1" s="24"/>
-      <c r="Q1" s="128">
+      <c r="Q1" s="127">
         <v>45656</v>
       </c>
-      <c r="R1" s="127"/>
-      <c r="S1" s="127"/>
-      <c r="T1" s="127"/>
-      <c r="U1" s="127"/>
-      <c r="V1" s="127"/>
-      <c r="W1" s="127"/>
-      <c r="X1" s="127"/>
-      <c r="Y1" s="127"/>
-      <c r="Z1" s="127"/>
+      <c r="R1" s="126"/>
+      <c r="S1" s="126"/>
+      <c r="T1" s="126"/>
+      <c r="U1" s="126"/>
+      <c r="V1" s="126"/>
+      <c r="W1" s="126"/>
+      <c r="X1" s="126"/>
+      <c r="Y1" s="126"/>
+      <c r="Z1" s="126"/>
     </row>
     <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B2" s="96" t="s">
@@ -1860,28 +1860,28 @@
       <c r="D2" s="22"/>
       <c r="E2" s="23"/>
       <c r="F2" s="22"/>
-      <c r="I2" s="129" t="s">
+      <c r="I2" s="128" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="130"/>
-      <c r="K2" s="130"/>
-      <c r="L2" s="130"/>
-      <c r="M2" s="130"/>
-      <c r="N2" s="130"/>
-      <c r="O2" s="130"/>
+      <c r="J2" s="129"/>
+      <c r="K2" s="129"/>
+      <c r="L2" s="129"/>
+      <c r="M2" s="129"/>
+      <c r="N2" s="129"/>
+      <c r="O2" s="129"/>
       <c r="P2" s="24"/>
-      <c r="Q2" s="126">
+      <c r="Q2" s="125">
         <v>1</v>
       </c>
-      <c r="R2" s="127"/>
-      <c r="S2" s="127"/>
-      <c r="T2" s="127"/>
-      <c r="U2" s="127"/>
-      <c r="V2" s="127"/>
-      <c r="W2" s="127"/>
-      <c r="X2" s="127"/>
-      <c r="Y2" s="127"/>
-      <c r="Z2" s="127"/>
+      <c r="R2" s="126"/>
+      <c r="S2" s="126"/>
+      <c r="T2" s="126"/>
+      <c r="U2" s="126"/>
+      <c r="V2" s="126"/>
+      <c r="W2" s="126"/>
+      <c r="X2" s="126"/>
+      <c r="Y2" s="126"/>
+      <c r="Z2" s="126"/>
     </row>
     <row r="3" spans="1:64" ht="25.2" x14ac:dyDescent="0.6">
       <c r="B3" s="96" t="s">
@@ -1975,102 +1975,102 @@
       <c r="A7" s="14"/>
       <c r="B7" s="29"/>
       <c r="E7" s="30"/>
-      <c r="I7" s="133">
+      <c r="I7" s="122">
         <f>I8</f>
         <v>45656</v>
       </c>
-      <c r="J7" s="131"/>
-      <c r="K7" s="131"/>
-      <c r="L7" s="131"/>
-      <c r="M7" s="131"/>
-      <c r="N7" s="131"/>
-      <c r="O7" s="131"/>
-      <c r="P7" s="131">
+      <c r="J7" s="120"/>
+      <c r="K7" s="120"/>
+      <c r="L7" s="120"/>
+      <c r="M7" s="120"/>
+      <c r="N7" s="120"/>
+      <c r="O7" s="120"/>
+      <c r="P7" s="120">
         <f>P8</f>
         <v>45663</v>
       </c>
-      <c r="Q7" s="131"/>
-      <c r="R7" s="131"/>
-      <c r="S7" s="131"/>
-      <c r="T7" s="131"/>
-      <c r="U7" s="131"/>
-      <c r="V7" s="131"/>
-      <c r="W7" s="131">
+      <c r="Q7" s="120"/>
+      <c r="R7" s="120"/>
+      <c r="S7" s="120"/>
+      <c r="T7" s="120"/>
+      <c r="U7" s="120"/>
+      <c r="V7" s="120"/>
+      <c r="W7" s="120">
         <f>W8</f>
         <v>45670</v>
       </c>
-      <c r="X7" s="131"/>
-      <c r="Y7" s="131"/>
-      <c r="Z7" s="131"/>
-      <c r="AA7" s="131"/>
-      <c r="AB7" s="131"/>
-      <c r="AC7" s="131"/>
-      <c r="AD7" s="131">
+      <c r="X7" s="120"/>
+      <c r="Y7" s="120"/>
+      <c r="Z7" s="120"/>
+      <c r="AA7" s="120"/>
+      <c r="AB7" s="120"/>
+      <c r="AC7" s="120"/>
+      <c r="AD7" s="120">
         <f>AD8</f>
         <v>45677</v>
       </c>
-      <c r="AE7" s="131"/>
-      <c r="AF7" s="131"/>
-      <c r="AG7" s="131"/>
-      <c r="AH7" s="131"/>
-      <c r="AI7" s="131"/>
-      <c r="AJ7" s="131"/>
-      <c r="AK7" s="131">
+      <c r="AE7" s="120"/>
+      <c r="AF7" s="120"/>
+      <c r="AG7" s="120"/>
+      <c r="AH7" s="120"/>
+      <c r="AI7" s="120"/>
+      <c r="AJ7" s="120"/>
+      <c r="AK7" s="120">
         <f>AK8</f>
         <v>45684</v>
       </c>
-      <c r="AL7" s="131"/>
-      <c r="AM7" s="131"/>
-      <c r="AN7" s="131"/>
-      <c r="AO7" s="131"/>
-      <c r="AP7" s="131"/>
-      <c r="AQ7" s="131"/>
-      <c r="AR7" s="131">
+      <c r="AL7" s="120"/>
+      <c r="AM7" s="120"/>
+      <c r="AN7" s="120"/>
+      <c r="AO7" s="120"/>
+      <c r="AP7" s="120"/>
+      <c r="AQ7" s="120"/>
+      <c r="AR7" s="120">
         <f>AR8</f>
         <v>45691</v>
       </c>
-      <c r="AS7" s="131"/>
-      <c r="AT7" s="131"/>
-      <c r="AU7" s="131"/>
-      <c r="AV7" s="131"/>
-      <c r="AW7" s="131"/>
-      <c r="AX7" s="131"/>
-      <c r="AY7" s="131">
+      <c r="AS7" s="120"/>
+      <c r="AT7" s="120"/>
+      <c r="AU7" s="120"/>
+      <c r="AV7" s="120"/>
+      <c r="AW7" s="120"/>
+      <c r="AX7" s="120"/>
+      <c r="AY7" s="120">
         <f>AY8</f>
         <v>45698</v>
       </c>
-      <c r="AZ7" s="131"/>
-      <c r="BA7" s="131"/>
-      <c r="BB7" s="131"/>
-      <c r="BC7" s="131"/>
-      <c r="BD7" s="131"/>
-      <c r="BE7" s="131"/>
-      <c r="BF7" s="131">
+      <c r="AZ7" s="120"/>
+      <c r="BA7" s="120"/>
+      <c r="BB7" s="120"/>
+      <c r="BC7" s="120"/>
+      <c r="BD7" s="120"/>
+      <c r="BE7" s="120"/>
+      <c r="BF7" s="120">
         <f>BF8</f>
         <v>45705</v>
       </c>
-      <c r="BG7" s="131"/>
-      <c r="BH7" s="131"/>
-      <c r="BI7" s="131"/>
-      <c r="BJ7" s="131"/>
-      <c r="BK7" s="131"/>
-      <c r="BL7" s="132"/>
+      <c r="BG7" s="120"/>
+      <c r="BH7" s="120"/>
+      <c r="BI7" s="120"/>
+      <c r="BJ7" s="120"/>
+      <c r="BK7" s="120"/>
+      <c r="BL7" s="121"/>
     </row>
     <row r="8" spans="1:64" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="120"/>
-      <c r="B8" s="121" t="s">
+      <c r="A8" s="130"/>
+      <c r="B8" s="131" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="123" t="s">
+      <c r="C8" s="133" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="125" t="s">
+      <c r="D8" s="123" t="s">
         <v>1</v>
       </c>
-      <c r="E8" s="125" t="s">
+      <c r="E8" s="123" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="125" t="s">
+      <c r="F8" s="123" t="s">
         <v>4</v>
       </c>
       <c r="I8" s="31">
@@ -2299,8 +2299,8 @@
       </c>
     </row>
     <row r="9" spans="1:64" s="26" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="120"/>
-      <c r="B9" s="122"/>
+      <c r="A9" s="130"/>
+      <c r="B9" s="132"/>
       <c r="C9" s="124"/>
       <c r="D9" s="124"/>
       <c r="E9" s="124"/>
@@ -2680,7 +2680,7 @@
         <v>48</v>
       </c>
       <c r="D12" s="49">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E12" s="50">
         <f>Project_Start</f>
@@ -2761,7 +2761,7 @@
         <v>49</v>
       </c>
       <c r="D13" s="54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="55">
         <f>F12</f>
@@ -2842,7 +2842,7 @@
         <v>50</v>
       </c>
       <c r="D14" s="54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="55">
         <f>F13</f>
@@ -2923,7 +2923,7 @@
         <v>51</v>
       </c>
       <c r="D15" s="54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" s="55">
         <f>F14</f>
@@ -3085,7 +3085,7 @@
         <v>50</v>
       </c>
       <c r="D18" s="64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" s="65">
         <f>F14+1</f>
@@ -3163,10 +3163,10 @@
         <v>30</v>
       </c>
       <c r="C19" s="63" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D19" s="64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="65">
         <f>F18</f>
@@ -3247,7 +3247,7 @@
         <v>48</v>
       </c>
       <c r="D20" s="64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="65">
         <f>F19</f>
@@ -3343,7 +3343,7 @@
         <v>48</v>
       </c>
       <c r="D22" s="116">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="E22" s="117">
         <f>F20+20</f>
@@ -3424,7 +3424,7 @@
         <v>50</v>
       </c>
       <c r="D23" s="116">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="E23" s="117">
         <f>E22+2</f>
@@ -4799,6 +4799,16 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="Q2:Z2"/>
+    <mergeCell ref="Q1:Z1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="I2:O2"/>
     <mergeCell ref="BF7:BL7"/>
     <mergeCell ref="I7:O7"/>
     <mergeCell ref="P7:V7"/>
@@ -4807,16 +4817,6 @@
     <mergeCell ref="AK7:AQ7"/>
     <mergeCell ref="AR7:AX7"/>
     <mergeCell ref="AY7:BE7"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="Q2:Z2"/>
-    <mergeCell ref="Q1:Z1"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="I2:O2"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
   </mergeCells>
   <conditionalFormatting sqref="D10:D39">
     <cfRule type="dataBar" priority="23">
@@ -5046,35 +5046,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="28" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="60f5a4f2d2b0abadcf532d48ebf9cb71">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7dd78129e6a1811f84807ad11c651531" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5386,34 +5357,36 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A09426A3-87E9-4865-8A6C-3456B026AE03}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5434,6 +5407,33 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata"/>
 </file>
</xml_diff>